<commit_message>
Updated technical provision notes
</commit_message>
<xml_diff>
--- a/documents/Dec24 MICL MI Pack v9.4 PL-BS.xlsx
+++ b/documents/Dec24 MICL MI Pack v9.4 PL-BS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.ciocoiu\Documents\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\Desktop\mul_doc\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3223DA-1190-4374-AEB9-06E87B82D909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84165B91-3504-48A5-A88F-9ED4CD758173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="405" windowWidth="24015" windowHeight="13800" tabRatio="870" firstSheet="3" activeTab="4" xr2:uid="{87E971D6-A8E9-4032-AAB6-94B3E81615F7}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="13515" tabRatio="870" firstSheet="3" activeTab="3" xr2:uid="{87E971D6-A8E9-4032-AAB6-94B3E81615F7}"/>
   </bookViews>
   <sheets>
     <sheet name="PL GFSC old" sheetId="28" state="hidden" r:id="rId1"/>
@@ -2856,24 +2856,24 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="18">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="#,##0;[Red]\(#,##0\);\-"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0;[Red]\(#,##0.0\);\-"/>
-    <numFmt numFmtId="170" formatCode="0.0%;[Red]\(0.0%\)"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00;[Red]\(#,##0.00\)"/>
-    <numFmt numFmtId="172" formatCode="mmmm\ yyyy"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00;[Red]\(#,##0.00\);\-"/>
-    <numFmt numFmtId="174" formatCode="#,##0;[Red]\(#,##0\)"/>
-    <numFmt numFmtId="175" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="#,##0;\(#,##0\);\-"/>
-    <numFmt numFmtId="177" formatCode="mmmm\ yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00;\(#,##0.00\);\-"/>
-    <numFmt numFmtId="179" formatCode="0.000"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0;[Red]\(#,##0\);\-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0;[Red]\(#,##0.0\);\-"/>
+    <numFmt numFmtId="167" formatCode="0.0%;[Red]\(0.0%\)"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00;[Red]\(#,##0.00\)"/>
+    <numFmt numFmtId="169" formatCode="mmmm\ yyyy"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00;[Red]\(#,##0.00\);\-"/>
+    <numFmt numFmtId="171" formatCode="#,##0;[Red]\(#,##0\)"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="173" formatCode="#,##0;\(#,##0\);\-"/>
+    <numFmt numFmtId="174" formatCode="mmmm\ yyyy;@"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00;\(#,##0.00\);\-"/>
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="60" x14ac:knownFonts="1">
     <font>
@@ -3875,14 +3875,14 @@
   <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -3927,28 +3927,28 @@
     <xf numFmtId="0" fontId="45" fillId="36" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="45" fillId="36" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3957,50 +3957,50 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4009,45 +4009,45 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="11" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="15" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="15" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="15" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="16" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4061,92 +4061,92 @@
     <xf numFmtId="0" fontId="27" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="27" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="27" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="168" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4156,56 +4156,56 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="29" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="27" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="27" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="53" applyFont="1"/>
-    <xf numFmtId="167" fontId="50" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="43" fontId="50" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="50" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="50" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="53" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="53" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="53" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4220,10 +4220,10 @@
     <xf numFmtId="17" fontId="55" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="55" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="55" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="55" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="55" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="53" applyFont="1" applyAlignment="1">
@@ -4235,20 +4235,20 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="28" xfId="53" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="50" fillId="0" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="50" fillId="0" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="50" fillId="0" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="50" fillId="0" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="53" applyFont="1"/>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="53" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="53" applyFont="1"/>
@@ -4256,7 +4256,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="37" borderId="0" xfId="53" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="50" fillId="3" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="50" fillId="3" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="53" applyFont="1" applyAlignment="1">
@@ -4265,107 +4265,107 @@
     <xf numFmtId="17" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="57" fillId="0" borderId="29" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="57" fillId="0" borderId="29" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="55" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="55" fillId="2" borderId="26" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="3" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="3" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="57" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="57" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="2" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="2" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="53" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="15" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="15" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="53" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="31" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="31" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="3" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="3" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="30" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="173" fontId="50" fillId="3" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="50" fillId="3" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="49" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="59" fillId="3" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="49" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="59" fillId="3" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="56" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="53" fillId="2" borderId="25" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="56" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="53" fillId="2" borderId="25" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="49" fillId="0" borderId="6" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="49" fillId="0" borderId="6" xfId="53" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="49" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="49" fillId="0" borderId="33" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="50" fillId="4" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="50" fillId="4" borderId="28" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="32" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="175" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="22" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="29" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4808,8 +4808,8 @@
       <xdr:rowOff>31040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>840483</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>2283</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>189291</xdr:rowOff>
     </xdr:to>
@@ -12354,11 +12354,11 @@
   </sheetPr>
   <dimension ref="A1:AH172"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A170" sqref="A170:XFD170"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -12536,7 +12536,7 @@
         <v>-17534.480960000001</v>
       </c>
     </row>
-    <row r="10" spans="1:34" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>5001</v>
       </c>
@@ -12571,7 +12571,7 @@
         <v>-17534.480960000001</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D11" s="68"/>
       <c r="E11" s="68"/>
       <c r="F11" s="68"/>
@@ -12584,7 +12584,7 @@
       <c r="M11" s="68"/>
       <c r="N11" s="68"/>
     </row>
-    <row r="12" spans="1:34" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
         <v>11</v>
       </c>
@@ -12619,7 +12619,7 @@
         <v>5614.177070000007</v>
       </c>
     </row>
-    <row r="13" spans="1:34" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>5010</v>
       </c>
@@ -12653,7 +12653,7 @@
         <v>9450.6926000000094</v>
       </c>
     </row>
-    <row r="14" spans="1:34" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>5011</v>
       </c>
@@ -12687,7 +12687,7 @@
         <v>-3242.5580700000028</v>
       </c>
     </row>
-    <row r="15" spans="1:34" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>5012</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>-593.95745999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="3.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="96"/>
       <c r="E16" s="96"/>
       <c r="F16" s="96"/>
@@ -12805,7 +12805,7 @@
         <v>-51549.215690000019</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46">
         <v>5020</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>-52396.875350000009</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="46">
         <v>5021</v>
       </c>
@@ -12873,7 +12873,7 @@
         <v>847.65965999999025</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
       <c r="F21" s="68"/>
@@ -12886,7 +12886,7 @@
       <c r="M21" s="68"/>
       <c r="N21" s="68"/>
     </row>
-    <row r="22" spans="1:14" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
         <v>11</v>
       </c>
@@ -12921,7 +12921,7 @@
         <v>45540.099680000007</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46">
         <v>5030</v>
       </c>
@@ -12955,7 +12955,7 @@
         <v>42346.022750000004</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="46">
         <v>5031</v>
       </c>
@@ -12989,7 +12989,7 @@
         <v>-823.94068999999581</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="46">
         <v>5034</v>
       </c>
@@ -13023,7 +13023,7 @@
         <v>-2866.518</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="46">
         <v>5035</v>
       </c>
@@ -13057,7 +13057,7 @@
         <v>108.7903</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46">
         <v>5032</v>
       </c>
@@ -13091,7 +13091,7 @@
         <v>6894.342349999999</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="46">
         <v>5033</v>
       </c>
@@ -13125,7 +13125,7 @@
         <v>-118.5970299999999</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D29" s="68"/>
       <c r="E29" s="68"/>
       <c r="F29" s="68"/>
@@ -13138,7 +13138,7 @@
       <c r="M29" s="68"/>
       <c r="N29" s="68"/>
     </row>
-    <row r="30" spans="1:14" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="61" t="s">
         <v>0</v>
       </c>
@@ -13171,7 +13171,7 @@
         <v>-17929.419900000008</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D31" s="68"/>
       <c r="E31" s="68"/>
       <c r="F31" s="68"/>
@@ -13184,7 +13184,7 @@
       <c r="M31" s="68"/>
       <c r="N31" s="68"/>
     </row>
-    <row r="32" spans="1:14" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A32" s="46">
         <v>5013</v>
       </c>
@@ -13219,7 +13219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="46">
         <v>5014</v>
       </c>
@@ -13254,7 +13254,7 @@
         <v>-326.63744000000042</v>
       </c>
     </row>
-    <row r="34" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="46">
         <v>5212</v>
       </c>
@@ -13288,7 +13288,7 @@
         <v>259.54415999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D35" s="68"/>
       <c r="E35" s="68"/>
       <c r="F35" s="68"/>
@@ -13300,7 +13300,7 @@
       <c r="M35" s="68"/>
       <c r="N35" s="68"/>
     </row>
-    <row r="36" spans="1:14" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="61" t="s">
         <v>346</v>
       </c>
@@ -13651,7 +13651,7 @@
         <v>19580.293610000001</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="46">
         <v>5401</v>
       </c>
@@ -13685,7 +13685,7 @@
         <v>19741.122770000002</v>
       </c>
     </row>
-    <row r="50" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="46">
         <v>5402</v>
       </c>
@@ -13719,7 +13719,7 @@
         <v>44.745840000000044</v>
       </c>
     </row>
-    <row r="51" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="46">
         <v>5403</v>
       </c>
@@ -13753,7 +13753,7 @@
         <v>-205.57499999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D52" s="68"/>
       <c r="E52" s="68"/>
       <c r="F52" s="68"/>
@@ -13766,7 +13766,7 @@
       <c r="M52" s="68"/>
       <c r="N52" s="68"/>
     </row>
-    <row r="53" spans="1:14" ht="3.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D53" s="68"/>
       <c r="E53" s="68"/>
       <c r="F53" s="68"/>
@@ -13814,7 +13814,7 @@
         <v>-13353.211289999992</v>
       </c>
     </row>
-    <row r="55" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="46">
         <v>5410</v>
       </c>
@@ -13848,7 +13848,7 @@
         <v>-13353.211289999992</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D56" s="68"/>
       <c r="E56" s="68"/>
       <c r="F56" s="68"/>
@@ -13861,7 +13861,7 @@
       <c r="M56" s="68"/>
       <c r="N56" s="68"/>
     </row>
-    <row r="57" spans="1:14" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="46" t="s">
         <v>14</v>
       </c>
@@ -13915,7 +13915,7 @@
         <v>67287.463299999989</v>
       </c>
     </row>
-    <row r="59" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="46">
         <v>5420</v>
       </c>
@@ -13949,7 +13949,7 @@
         <v>54337.704360000003</v>
       </c>
     </row>
-    <row r="60" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="46">
         <v>5421</v>
       </c>
@@ -13983,7 +13983,7 @@
         <v>9664.8724599999841</v>
       </c>
     </row>
-    <row r="61" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="46">
         <v>5422</v>
       </c>
@@ -14017,7 +14017,7 @@
         <v>13570.278410000003</v>
       </c>
     </row>
-    <row r="62" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="46">
         <v>5423</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>-8733.4370699999963</v>
       </c>
     </row>
-    <row r="63" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="46">
         <v>5424</v>
       </c>
@@ -14085,7 +14085,7 @@
         <v>-1590.5589799999998</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="46">
         <v>5425</v>
       </c>
@@ -14119,7 +14119,7 @@
         <v>38.604120000000016</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D65" s="68"/>
       <c r="E65" s="68"/>
       <c r="F65" s="68"/>
@@ -14132,7 +14132,7 @@
       <c r="M65" s="68"/>
       <c r="N65" s="68"/>
     </row>
-    <row r="66" spans="1:14" ht="3.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D66" s="68"/>
       <c r="E66" s="68"/>
       <c r="F66" s="68"/>
@@ -14180,7 +14180,7 @@
         <v>-58178.656830000022</v>
       </c>
     </row>
-    <row r="68" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="46">
         <v>5430</v>
       </c>
@@ -14215,7 +14215,7 @@
         <v>-18464.991160000005</v>
       </c>
     </row>
-    <row r="69" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="46">
         <v>5431</v>
       </c>
@@ -14250,7 +14250,7 @@
         <v>310.92744999999559</v>
       </c>
     </row>
-    <row r="70" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="46">
         <v>5432</v>
       </c>
@@ -14284,7 +14284,7 @@
         <v>-27214.340540000005</v>
       </c>
     </row>
-    <row r="71" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="46">
         <v>5433</v>
       </c>
@@ -14318,7 +14318,7 @@
         <v>1356.7247699999862</v>
       </c>
     </row>
-    <row r="72" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="46">
         <v>5434</v>
       </c>
@@ -14352,7 +14352,7 @@
         <v>-15174.175629999998</v>
       </c>
     </row>
-    <row r="73" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="46">
         <v>5435</v>
       </c>
@@ -14386,7 +14386,7 @@
         <v>1007.1982800000005</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D74" s="68"/>
       <c r="E74" s="68"/>
       <c r="F74" s="68"/>
@@ -14399,7 +14399,7 @@
       <c r="M74" s="68"/>
       <c r="N74" s="68"/>
     </row>
-    <row r="75" spans="1:14" ht="3.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D75" s="68"/>
       <c r="E75" s="68"/>
       <c r="F75" s="68"/>
@@ -14496,7 +14496,7 @@
         <v>-16688.435129999998</v>
       </c>
     </row>
-    <row r="79" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="46">
         <v>6001</v>
       </c>
@@ -14530,7 +14530,7 @@
         <v>3358.3206099999998</v>
       </c>
     </row>
-    <row r="80" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="46">
         <v>6002</v>
       </c>
@@ -14564,7 +14564,7 @@
         <v>-9004.7332299999998</v>
       </c>
     </row>
-    <row r="81" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="46">
         <v>6003</v>
       </c>
@@ -14598,7 +14598,7 @@
         <v>10147.525390000001</v>
       </c>
     </row>
-    <row r="82" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="46">
         <v>6004</v>
       </c>
@@ -14632,7 +14632,7 @@
         <v>-354.98623000000043</v>
       </c>
     </row>
-    <row r="83" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="46">
         <v>6005</v>
       </c>
@@ -14666,7 +14666,7 @@
         <v>-9217.3381300000001</v>
       </c>
     </row>
-    <row r="84" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="46">
         <v>6006</v>
       </c>
@@ -14700,7 +14700,7 @@
         <v>3097.4196199999997</v>
       </c>
     </row>
-    <row r="85" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="46">
         <v>6010</v>
       </c>
@@ -14734,7 +14734,7 @@
         <v>-663.51377999999977</v>
       </c>
     </row>
-    <row r="86" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="46">
         <v>6012</v>
       </c>
@@ -14768,7 +14768,7 @@
         <v>248.50152000000003</v>
       </c>
     </row>
-    <row r="87" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="46">
         <v>6013</v>
       </c>
@@ -14802,7 +14802,7 @@
         <v>415.90323000000012</v>
       </c>
     </row>
-    <row r="88" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="46">
         <v>6020</v>
       </c>
@@ -14836,7 +14836,7 @@
         <v>4625.0857099999994</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="46">
         <v>6023</v>
       </c>
@@ -14870,7 +14870,7 @@
         <v>-485.99949000000004</v>
       </c>
     </row>
-    <row r="90" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="46">
         <v>6021</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>-29.75958</v>
       </c>
     </row>
-    <row r="91" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="46">
         <v>6240</v>
       </c>
@@ -14938,7 +14938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="46">
         <v>5201</v>
       </c>
@@ -14972,7 +14972,7 @@
         <v>-538.35092999999995</v>
       </c>
     </row>
-    <row r="93" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="46">
         <v>5202</v>
       </c>
@@ -15006,7 +15006,7 @@
         <v>95.092820000000017</v>
       </c>
     </row>
-    <row r="94" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="46">
         <v>8301</v>
       </c>
@@ -15040,7 +15040,7 @@
         <v>0.34155999999999942</v>
       </c>
     </row>
-    <row r="95" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="46">
         <v>8602</v>
       </c>
@@ -15074,7 +15074,7 @@
         <v>-1050.6567700000001</v>
       </c>
     </row>
-    <row r="96" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="46">
         <v>8608</v>
       </c>
@@ -15108,7 +15108,7 @@
         <v>-146.71201000000002</v>
       </c>
     </row>
-    <row r="97" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="46">
         <v>8603</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>560.38596999999993</v>
       </c>
     </row>
-    <row r="98" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="46">
         <v>8601</v>
       </c>
@@ -15176,7 +15176,7 @@
         <v>65.940010000000029</v>
       </c>
     </row>
-    <row r="99" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="46">
         <v>8114</v>
       </c>
@@ -15210,7 +15210,7 @@
         <v>3.7296</v>
       </c>
     </row>
-    <row r="100" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="46">
         <v>7200</v>
       </c>
@@ -15244,7 +15244,7 @@
         <v>-21.354939999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="46">
         <v>7101</v>
       </c>
@@ -15278,7 +15278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="46">
         <v>8332</v>
       </c>
@@ -15312,7 +15312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="46">
         <v>8012</v>
       </c>
@@ -15346,7 +15346,7 @@
         <v>-0.59301999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="46">
         <v>8117</v>
       </c>
@@ -15380,7 +15380,7 @@
         <v>-32.849730000000022</v>
       </c>
     </row>
-    <row r="105" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="46">
         <v>8530</v>
       </c>
@@ -15414,7 +15414,7 @@
         <v>-2510.4245600000004</v>
       </c>
     </row>
-    <row r="106" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="46">
         <v>8020</v>
       </c>
@@ -15448,7 +15448,7 @@
         <v>-19.213830000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="46">
         <v>8401</v>
       </c>
@@ -15482,7 +15482,7 @@
         <v>-34.676419999999993</v>
       </c>
     </row>
-    <row r="108" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="46">
         <v>8120</v>
       </c>
@@ -15516,7 +15516,7 @@
         <v>-65.390179999999987</v>
       </c>
     </row>
-    <row r="109" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="46">
         <v>5203</v>
       </c>
@@ -15550,7 +15550,7 @@
         <v>158.86471999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="46">
         <v>5204</v>
       </c>
@@ -15584,7 +15584,7 @@
         <v>43.532820000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A111" s="46">
         <v>8511</v>
       </c>
@@ -15618,7 +15618,7 @@
         <v>66.932649999999967</v>
       </c>
     </row>
-    <row r="112" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="46">
         <v>8440</v>
       </c>
@@ -15652,7 +15652,7 @@
         <v>-34.416929999999994</v>
       </c>
     </row>
-    <row r="113" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" s="46">
         <v>8250</v>
       </c>
@@ -15686,7 +15686,7 @@
         <v>-14750.331269999999</v>
       </c>
     </row>
-    <row r="114" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="46">
         <v>8604</v>
       </c>
@@ -15720,7 +15720,7 @@
         <v>-258.29744999999997</v>
       </c>
     </row>
-    <row r="115" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" s="46">
         <v>8512</v>
       </c>
@@ -15754,7 +15754,7 @@
         <v>-359.40469999999982</v>
       </c>
     </row>
-    <row r="116" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" s="46">
         <v>8702</v>
       </c>
@@ -15788,7 +15788,7 @@
         <v>-47.76446</v>
       </c>
     </row>
-    <row r="117" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="46">
         <v>8701</v>
       </c>
@@ -15822,7 +15822,7 @@
         <v>50.756279999999997</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D118" s="68"/>
       <c r="E118" s="68"/>
       <c r="F118" s="68"/>
@@ -15835,7 +15835,7 @@
       <c r="M118" s="68"/>
       <c r="N118" s="68"/>
     </row>
-    <row r="119" spans="1:14" ht="3.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D119" s="68"/>
       <c r="E119" s="68"/>
       <c r="F119" s="68"/>
@@ -15883,7 +15883,7 @@
         <v>2312.4621899999997</v>
       </c>
     </row>
-    <row r="121" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A121" s="46" t="s">
         <v>11</v>
       </c>
@@ -15918,7 +15918,7 @@
         <v>861.13193999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A122" s="46">
         <v>9001</v>
       </c>
@@ -15952,7 +15952,7 @@
         <v>591.02449000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A123" s="46">
         <v>9201</v>
       </c>
@@ -15986,7 +15986,7 @@
         <v>196.82515000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A124" s="46">
         <v>9400</v>
       </c>
@@ -16020,7 +16020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A125" s="46">
         <v>9410</v>
       </c>
@@ -16054,7 +16054,7 @@
         <v>283.17200000000003</v>
       </c>
     </row>
-    <row r="126" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A126" s="46">
         <v>9430</v>
       </c>
@@ -16088,7 +16088,7 @@
         <v>608.35908999999992</v>
       </c>
     </row>
-    <row r="127" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A127" s="46">
         <v>9450</v>
       </c>
@@ -16122,7 +16122,7 @@
         <v>-223.25814999999994</v>
       </c>
     </row>
-    <row r="128" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A128" s="46">
         <v>9451</v>
       </c>
@@ -16156,7 +16156,7 @@
         <v>1.5559099999999972</v>
       </c>
     </row>
-    <row r="129" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A129" s="46">
         <v>9453</v>
       </c>
@@ -16190,7 +16190,7 @@
         <v>62.070399999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A130" s="46">
         <v>9454</v>
       </c>
@@ -16224,7 +16224,7 @@
         <v>-377.90243000000004</v>
       </c>
     </row>
-    <row r="131" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A131" s="46">
         <v>9455</v>
       </c>
@@ -16258,7 +16258,7 @@
         <v>-280.71451999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A132" s="46">
         <v>9452</v>
       </c>
@@ -16292,7 +16292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="3.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D133" s="68"/>
       <c r="E133" s="68"/>
       <c r="F133" s="68"/>
@@ -16305,7 +16305,7 @@
       <c r="M133" s="68"/>
       <c r="N133" s="68"/>
     </row>
-    <row r="134" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D134" s="68"/>
       <c r="E134" s="68"/>
       <c r="F134" s="68"/>
@@ -16318,7 +16318,7 @@
       <c r="M134" s="68"/>
       <c r="N134" s="68"/>
     </row>
-    <row r="135" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A135" s="46" t="s">
         <v>11</v>
       </c>
@@ -16353,7 +16353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A136" s="46">
         <v>9423</v>
       </c>
@@ -16388,7 +16388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D137" s="68"/>
       <c r="E137" s="68"/>
       <c r="F137" s="68"/>
@@ -16401,7 +16401,7 @@
       <c r="M137" s="68"/>
       <c r="N137" s="68"/>
     </row>
-    <row r="138" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A138" s="46" t="s">
         <v>11</v>
       </c>
@@ -16436,7 +16436,7 @@
         <v>312.95913999999982</v>
       </c>
     </row>
-    <row r="139" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A139" s="46">
         <v>9403</v>
       </c>
@@ -16470,7 +16470,7 @@
         <v>-2247.4527900000003</v>
       </c>
     </row>
-    <row r="140" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A140" s="46">
         <v>9432</v>
       </c>
@@ -16504,7 +16504,7 @@
         <v>2631.62309</v>
       </c>
     </row>
-    <row r="141" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A141" s="46">
         <v>9434</v>
       </c>
@@ -16538,7 +16538,7 @@
         <v>37.991510000000005</v>
       </c>
     </row>
-    <row r="142" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A142" s="46">
         <v>9442</v>
       </c>
@@ -16572,7 +16572,7 @@
         <v>13.315529999999995</v>
       </c>
     </row>
-    <row r="143" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A143" s="46">
         <v>9413</v>
       </c>
@@ -16606,7 +16606,7 @@
         <v>-122.51819999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="3.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D144" s="68"/>
       <c r="E144" s="68"/>
       <c r="F144" s="68"/>
@@ -16619,7 +16619,7 @@
       <c r="M144" s="68"/>
       <c r="N144" s="68"/>
     </row>
-    <row r="145" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A145" s="46" t="s">
         <v>11</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>1176.01956</v>
       </c>
     </row>
-    <row r="146" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A146" s="46">
         <v>9501</v>
       </c>
@@ -16688,7 +16688,7 @@
         <v>1176.01956</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="3.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D147" s="68"/>
       <c r="E147" s="68"/>
       <c r="F147" s="68"/>
@@ -16701,7 +16701,7 @@
       <c r="M147" s="68"/>
       <c r="N147" s="68"/>
     </row>
-    <row r="148" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A148" s="46" t="s">
         <v>11</v>
       </c>
@@ -16736,7 +16736,7 @@
         <v>-37.648449999999997</v>
       </c>
     </row>
-    <row r="149" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A149" s="46">
         <v>9480</v>
       </c>
@@ -16770,7 +16770,7 @@
         <v>-45.016489999999997</v>
       </c>
     </row>
-    <row r="150" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A150" s="46">
         <v>9481</v>
       </c>
@@ -16804,7 +16804,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="151" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A151" s="46">
         <v>9482</v>
       </c>
@@ -16838,7 +16838,7 @@
         <v>18.368040000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="3.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="D152" s="68"/>
       <c r="E152" s="68"/>
       <c r="F152" s="68"/>
@@ -16851,7 +16851,7 @@
       <c r="M152" s="68"/>
       <c r="N152" s="68"/>
     </row>
-    <row r="153" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A153" s="46" t="s">
         <v>11</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A154" s="46">
         <v>9401</v>
       </c>
@@ -16920,7 +16920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="3.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="3.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D155" s="68"/>
       <c r="E155" s="68"/>
       <c r="F155" s="68"/>
@@ -16933,7 +16933,7 @@
       <c r="M155" s="68"/>
       <c r="N155" s="68"/>
     </row>
-    <row r="156" spans="1:14" ht="3.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D156" s="96"/>
       <c r="E156" s="96"/>
       <c r="F156" s="96"/>
@@ -17080,7 +17080,7 @@
       </c>
       <c r="O161" s="72"/>
     </row>
-    <row r="162" spans="1:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B162" s="46" t="s">
         <v>23</v>
       </c>
@@ -17112,7 +17112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:15" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C163" s="56"/>
       <c r="E163" s="56"/>
       <c r="F163" s="56"/>
@@ -17122,7 +17122,7 @@
       <c r="L163" s="56"/>
       <c r="N163" s="56"/>
     </row>
-    <row r="164" spans="1:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B164" s="70" t="s">
         <v>30</v>
       </c>
@@ -17133,7 +17133,7 @@
       <c r="K164" s="56"/>
       <c r="N164" s="56"/>
     </row>
-    <row r="165" spans="1:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B165" s="46" t="s">
         <v>31</v>
       </c>
@@ -17163,7 +17163,7 @@
         <v>5.6177329765002004E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B166" s="46" t="s">
         <v>32</v>
       </c>
@@ -17193,7 +17193,7 @@
         <v>-1.0523205720006845E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B167" s="46" t="s">
         <v>33</v>
       </c>
@@ -17223,7 +17223,7 @@
         <v>-5.4785647633923004E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B168" s="46" t="s">
         <v>34</v>
       </c>
@@ -17253,7 +17253,7 @@
         <v>1.6613738568485015E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:15" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B169" s="46" t="s">
         <v>35</v>
       </c>
@@ -17283,7 +17283,7 @@
         <v>-1.3562764193884334E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="200.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="165"/>
       <c r="C170" s="165"/>
       <c r="D170" s="166"/>
@@ -17342,11 +17342,11 @@
   </sheetPr>
   <dimension ref="A1:AG178"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J128" sqref="J128"/>
+      <selection pane="bottomRight" activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -21036,27 +21036,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="57e90656-23c1-4796-85cf-52b724a81a1a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b214f048-0a83-4059-9242-35dc8ddce195" xsi:nil="true"/>
-    <Month xmlns="57e90656-23c1-4796-85cf-52b724a81a1a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FB6F22F1EB776A4895D5B15BCEB3DD76" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7691b688df63e6b3f8679ce38aa5c6c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="57e90656-23c1-4796-85cf-52b724a81a1a" xmlns:ns3="b214f048-0a83-4059-9242-35dc8ddce195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b27e9b56b262a54c817e378c74b5a067" ns2:_="" ns3:_="">
     <xsd:import namespace="57e90656-23c1-4796-85cf-52b724a81a1a"/>
@@ -21291,32 +21270,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{445C3E41-B4B4-41A8-BFA0-56BA85673518}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b214f048-0a83-4059-9242-35dc8ddce195"/>
-    <ds:schemaRef ds:uri="57e90656-23c1-4796-85cf-52b724a81a1a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{294B137A-A5DB-45DB-8D42-D87B7C5DA140}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="57e90656-23c1-4796-85cf-52b724a81a1a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b214f048-0a83-4059-9242-35dc8ddce195" xsi:nil="true"/>
+    <Month xmlns="57e90656-23c1-4796-85cf-52b724a81a1a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B3DF4DD-2754-448E-AE11-55A3E0D7C88D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21335,6 +21310,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{294B137A-A5DB-45DB-8D42-D87B7C5DA140}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{445C3E41-B4B4-41A8-BFA0-56BA85673518}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b214f048-0a83-4059-9242-35dc8ddce195"/>
+    <ds:schemaRef ds:uri="57e90656-23c1-4796-85cf-52b724a81a1a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{4dcc80ff-3a52-4766-b76e-262847ecd459}" enabled="0" method="" siteId="{4dcc80ff-3a52-4766-b76e-262847ecd459}" removed="1"/>

</xml_diff>